<commit_message>
Adjust example Power_VRESProfiles to have ScenarioA and B
Update to latest InOutModule
</commit_message>
<xml_diff>
--- a/data/example/Power_VRESProfiles.xlsx
+++ b/data/example/Power_VRESProfiles.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\InOutModule\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F29B68A-1A10-44EF-AEB9-2ACE51114EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3767A690-3E57-4CC0-9894-396C949BA40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="scenario" sheetId="108" r:id="rId1"/>
+    <sheet name="ScenarioA" sheetId="108" r:id="rId1"/>
+    <sheet name="ScenarioB" sheetId="109" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="businfo">#REF!</definedName>
@@ -34,7 +35,8 @@
     <definedName name="network">#REF!</definedName>
     <definedName name="param">#REF!</definedName>
     <definedName name="renewable">#REF!</definedName>
-    <definedName name="resprofile">scenario!$C$3:$AD$36</definedName>
+    <definedName name="resprofile" localSheetId="1">ScenarioB!$C$3:$AD$36</definedName>
+    <definedName name="resprofile">ScenarioA!$C$3:$AD$36</definedName>
     <definedName name="runofriver">#REF!</definedName>
     <definedName name="sCodeName">#REF!</definedName>
     <definedName name="storage">#REF!</definedName>
@@ -141,8 +143,88 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Felix Auer</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{55F83AB3-2B81-4CCA-8C3B-5023B8439BA5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Readable Name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{6FF74646-CCF9-4B9F-9877-D091A917D055}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value specifier in DB</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{06C70B1A-FDB8-44A6-99B2-8B8205FAE6D2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Description</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{D90760BD-30D9-4FBE-9A28-3AE23488A339}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Details on database behavior</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{641996B5-8B1D-423F-8FE9-4F19DC27D235}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit or valid values</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="63">
   <si>
     <t>k0001</t>
   </si>
@@ -4399,10 +4481,3519 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44BD803-770F-4F3A-A452-AF6EFFC24E30}">
+  <sheetPr>
+    <tabColor rgb="FF008080"/>
+  </sheetPr>
+  <dimension ref="B1:AD63"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="29" width="8" style="2" customWidth="1"/>
+    <col min="30" max="16384" width="8" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:30" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="W4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="X4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD4" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="12"/>
+    </row>
+    <row r="6" spans="2:30" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="T6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="U6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="W6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="X6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD6" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+      <c r="C8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="16">
+        <v>0.28664138048556909</v>
+      </c>
+      <c r="H8" s="16">
+        <v>0.30204643249935381</v>
+      </c>
+      <c r="I8" s="16">
+        <v>0.29772660670507317</v>
+      </c>
+      <c r="J8" s="16">
+        <v>0.28185425836120215</v>
+      </c>
+      <c r="K8" s="16">
+        <v>0.28274974554827031</v>
+      </c>
+      <c r="L8" s="16">
+        <v>0.25346853923668322</v>
+      </c>
+      <c r="M8" s="16">
+        <v>0.24498166805221788</v>
+      </c>
+      <c r="N8" s="16">
+        <v>0.24144946807001441</v>
+      </c>
+      <c r="O8" s="16">
+        <v>0.21867331206565141</v>
+      </c>
+      <c r="P8" s="16">
+        <v>0.20626875384422511</v>
+      </c>
+      <c r="Q8" s="16">
+        <v>0.18773424017665566</v>
+      </c>
+      <c r="R8" s="16">
+        <v>0.19482093271085688</v>
+      </c>
+      <c r="S8" s="16">
+        <v>0.20379147583569832</v>
+      </c>
+      <c r="T8" s="16">
+        <v>0.20054139250844219</v>
+      </c>
+      <c r="U8" s="16">
+        <v>0.18576689753716766</v>
+      </c>
+      <c r="V8" s="16">
+        <v>0.17853167583049748</v>
+      </c>
+      <c r="W8" s="16">
+        <v>0.18054859187116845</v>
+      </c>
+      <c r="X8" s="16">
+        <v>0.18391281173120988</v>
+      </c>
+      <c r="Y8" s="16">
+        <v>0.21187319870015672</v>
+      </c>
+      <c r="Z8" s="16">
+        <v>0.21280806705444566</v>
+      </c>
+      <c r="AA8" s="16">
+        <v>0.20679724698996624</v>
+      </c>
+      <c r="AB8" s="16">
+        <v>0.23261862030937117</v>
+      </c>
+      <c r="AC8" s="16">
+        <v>0.22812088380183212</v>
+      </c>
+      <c r="AD8" s="16">
+        <v>0.24846629051067809</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+      <c r="C9" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0.11344605724313699</v>
+      </c>
+      <c r="H9" s="16">
+        <v>0.10931220235405539</v>
+      </c>
+      <c r="I9" s="16">
+        <v>0.10686470598243318</v>
+      </c>
+      <c r="J9" s="16">
+        <v>0.10678969767938072</v>
+      </c>
+      <c r="K9" s="16">
+        <v>9.8341679198297449E-2</v>
+      </c>
+      <c r="L9" s="16">
+        <v>0.10410621904577032</v>
+      </c>
+      <c r="M9" s="16">
+        <v>9.789113100094203E-2</v>
+      </c>
+      <c r="N9" s="16">
+        <v>9.1802358282215016E-2</v>
+      </c>
+      <c r="O9" s="16">
+        <v>8.9051655673551056E-2</v>
+      </c>
+      <c r="P9" s="16">
+        <v>9.351252767775374E-2</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>8.6446994769641197E-2</v>
+      </c>
+      <c r="R9" s="16">
+        <v>9.7404054204277543E-2</v>
+      </c>
+      <c r="S9" s="16">
+        <v>0.10261215248929142</v>
+      </c>
+      <c r="T9" s="16">
+        <v>0.12112397014179369</v>
+      </c>
+      <c r="U9" s="16">
+        <v>0.13453967222860644</v>
+      </c>
+      <c r="V9" s="16">
+        <v>0.14302936177914036</v>
+      </c>
+      <c r="W9" s="16">
+        <v>0.16055543365853667</v>
+      </c>
+      <c r="X9" s="16">
+        <v>0.16152198816366894</v>
+      </c>
+      <c r="Y9" s="16">
+        <v>0.16083573529844142</v>
+      </c>
+      <c r="Z9" s="16">
+        <v>0.14581503326702258</v>
+      </c>
+      <c r="AA9" s="16">
+        <v>0.13329572916363361</v>
+      </c>
+      <c r="AB9" s="16">
+        <v>0.12714073784551</v>
+      </c>
+      <c r="AC9" s="16">
+        <v>0.11951609833422287</v>
+      </c>
+      <c r="AD9" s="16">
+        <v>0.12173230288867264</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B10" s="14"/>
+      <c r="C10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0.14279196718905324</v>
+      </c>
+      <c r="H10" s="16">
+        <v>0.15998755015921964</v>
+      </c>
+      <c r="I10" s="16">
+        <v>0.15084346748365507</v>
+      </c>
+      <c r="J10" s="16">
+        <v>0.14693988493272286</v>
+      </c>
+      <c r="K10" s="16">
+        <v>0.14425316863534449</v>
+      </c>
+      <c r="L10" s="16">
+        <v>0.13323013820095336</v>
+      </c>
+      <c r="M10" s="16">
+        <v>0.12709990602999158</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0.1178778403255233</v>
+      </c>
+      <c r="O10" s="16">
+        <v>0.10927262393427742</v>
+      </c>
+      <c r="P10" s="16">
+        <v>0.10377572042801657</v>
+      </c>
+      <c r="Q10" s="16">
+        <v>0.10421440075447323</v>
+      </c>
+      <c r="R10" s="16">
+        <v>9.9404355743572037E-2</v>
+      </c>
+      <c r="S10" s="16">
+        <v>0.10456042270582672</v>
+      </c>
+      <c r="T10" s="16">
+        <v>0.1143217330488796</v>
+      </c>
+      <c r="U10" s="16">
+        <v>0.11882302773530425</v>
+      </c>
+      <c r="V10" s="16">
+        <v>0.13287487549247601</v>
+      </c>
+      <c r="W10" s="16">
+        <v>0.13367986349523631</v>
+      </c>
+      <c r="X10" s="16">
+        <v>0.14979740031289057</v>
+      </c>
+      <c r="Y10" s="16">
+        <v>0.15571909354869323</v>
+      </c>
+      <c r="Z10" s="16">
+        <v>0.14902720556125262</v>
+      </c>
+      <c r="AA10" s="16">
+        <v>0.15250973155562678</v>
+      </c>
+      <c r="AB10" s="16">
+        <v>0.14228115129660496</v>
+      </c>
+      <c r="AC10" s="16">
+        <v>0.15220536813768462</v>
+      </c>
+      <c r="AD10" s="16">
+        <v>0.16008822752094126</v>
+      </c>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B11" s="14"/>
+      <c r="C11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="16">
+        <v>0.51987086285737727</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0.56222800542994977</v>
+      </c>
+      <c r="I11" s="16">
+        <v>0.52275242402700228</v>
+      </c>
+      <c r="J11" s="16">
+        <v>0.52933992258625617</v>
+      </c>
+      <c r="K11" s="16">
+        <v>0.53190415046183637</v>
+      </c>
+      <c r="L11" s="16">
+        <v>0.51327220302133991</v>
+      </c>
+      <c r="M11" s="16">
+        <v>0.48106815142615073</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0.46241259307449745</v>
+      </c>
+      <c r="O11" s="16">
+        <v>0.46769142560427102</v>
+      </c>
+      <c r="P11" s="16">
+        <v>0.4769002567525264</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>0.43315519637472499</v>
+      </c>
+      <c r="R11" s="16">
+        <v>0.45891998854000748</v>
+      </c>
+      <c r="S11" s="16">
+        <v>0.41125529120431525</v>
+      </c>
+      <c r="T11" s="16">
+        <v>0.4144491408775588</v>
+      </c>
+      <c r="U11" s="16">
+        <v>0.36757221055865646</v>
+      </c>
+      <c r="V11" s="16">
+        <v>0.36482019353021944</v>
+      </c>
+      <c r="W11" s="16">
+        <v>0.34985205003641834</v>
+      </c>
+      <c r="X11" s="16">
+        <v>0.34771892893828588</v>
+      </c>
+      <c r="Y11" s="16">
+        <v>0.36496760702142583</v>
+      </c>
+      <c r="Z11" s="16">
+        <v>0.39095850146758276</v>
+      </c>
+      <c r="AA11" s="16">
+        <v>0.38687703520461664</v>
+      </c>
+      <c r="AB11" s="16">
+        <v>0.44718174681387612</v>
+      </c>
+      <c r="AC11" s="16">
+        <v>0.46449559414178554</v>
+      </c>
+      <c r="AD11" s="16">
+        <v>0.49231696260867958</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+      <c r="C12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="16">
+        <v>0.34369358475147482</v>
+      </c>
+      <c r="H12" s="16">
+        <v>0.3305241577378899</v>
+      </c>
+      <c r="I12" s="16">
+        <v>0.35045810808091449</v>
+      </c>
+      <c r="J12" s="16">
+        <v>0.36668770961990349</v>
+      </c>
+      <c r="K12" s="16">
+        <v>0.39036250286854762</v>
+      </c>
+      <c r="L12" s="16">
+        <v>0.36004467887238834</v>
+      </c>
+      <c r="M12" s="16">
+        <v>0.38619508632339961</v>
+      </c>
+      <c r="N12" s="16">
+        <v>0.39851623176319839</v>
+      </c>
+      <c r="O12" s="16">
+        <v>0.39735520779385086</v>
+      </c>
+      <c r="P12" s="16">
+        <v>0.41051148535890553</v>
+      </c>
+      <c r="Q12" s="16">
+        <v>0.46315378613794717</v>
+      </c>
+      <c r="R12" s="16">
+        <v>0.4557104436465827</v>
+      </c>
+      <c r="S12" s="16">
+        <v>0.4603659366042695</v>
+      </c>
+      <c r="T12" s="16">
+        <v>0.48994856285145072</v>
+      </c>
+      <c r="U12" s="16">
+        <v>0.4803101368492656</v>
+      </c>
+      <c r="V12" s="16">
+        <v>0.4558362676633983</v>
+      </c>
+      <c r="W12" s="16">
+        <v>0.39334819718104552</v>
+      </c>
+      <c r="X12" s="16">
+        <v>0.36254907055693075</v>
+      </c>
+      <c r="Y12" s="16">
+        <v>0.34764154401045561</v>
+      </c>
+      <c r="Z12" s="16">
+        <v>0.32026556339028056</v>
+      </c>
+      <c r="AA12" s="16">
+        <v>0.28788380543779685</v>
+      </c>
+      <c r="AB12" s="16">
+        <v>0.27836330449441715</v>
+      </c>
+      <c r="AC12" s="16">
+        <v>0.29075755034167844</v>
+      </c>
+      <c r="AD12" s="16">
+        <v>0.282396808464417</v>
+      </c>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="16">
+        <v>0.53952177813367674</v>
+      </c>
+      <c r="H13" s="16">
+        <v>0.55358204612882111</v>
+      </c>
+      <c r="I13" s="16">
+        <v>0.58636278173578826</v>
+      </c>
+      <c r="J13" s="16">
+        <v>0.61078136688331075</v>
+      </c>
+      <c r="K13" s="16">
+        <v>0.61968280637777529</v>
+      </c>
+      <c r="L13" s="16">
+        <v>0.59230076639291096</v>
+      </c>
+      <c r="M13" s="16">
+        <v>0.61065852474788396</v>
+      </c>
+      <c r="N13" s="16">
+        <v>0.60089890152433822</v>
+      </c>
+      <c r="O13" s="16">
+        <v>0.57701992423282189</v>
+      </c>
+      <c r="P13" s="16">
+        <v>0.60215653277331982</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>0.61579725923038053</v>
+      </c>
+      <c r="R13" s="16">
+        <v>0.63579559320809642</v>
+      </c>
+      <c r="S13" s="16">
+        <v>0.65108830415785979</v>
+      </c>
+      <c r="T13" s="16">
+        <v>0.66093816407819894</v>
+      </c>
+      <c r="U13" s="16">
+        <v>0.67831944544846101</v>
+      </c>
+      <c r="V13" s="16">
+        <v>0.70437080232479954</v>
+      </c>
+      <c r="W13" s="16">
+        <v>0.6901173724383729</v>
+      </c>
+      <c r="X13" s="16">
+        <v>0.6839579337868219</v>
+      </c>
+      <c r="Y13" s="16">
+        <v>0.67688512300044568</v>
+      </c>
+      <c r="Z13" s="16">
+        <v>0.63794261059520008</v>
+      </c>
+      <c r="AA13" s="16">
+        <v>0.62278559060940208</v>
+      </c>
+      <c r="AB13" s="16">
+        <v>0.59662709926711255</v>
+      </c>
+      <c r="AC13" s="16">
+        <v>0.58346585914364568</v>
+      </c>
+      <c r="AD13" s="16">
+        <v>0.58302547181083897</v>
+      </c>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B14" s="14"/>
+      <c r="C14" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0.67375188320215373</v>
+      </c>
+      <c r="H14" s="16">
+        <v>0.71761561088178105</v>
+      </c>
+      <c r="I14" s="16">
+        <v>0.66798065932728212</v>
+      </c>
+      <c r="J14" s="16">
+        <v>0.70861030050948792</v>
+      </c>
+      <c r="K14" s="16">
+        <v>0.70427181090647051</v>
+      </c>
+      <c r="L14" s="16">
+        <v>0.75908720973419197</v>
+      </c>
+      <c r="M14" s="16">
+        <v>0.75311422345335544</v>
+      </c>
+      <c r="N14" s="16">
+        <v>0.76400321508224867</v>
+      </c>
+      <c r="O14" s="16">
+        <v>0.74364035238831394</v>
+      </c>
+      <c r="P14" s="16">
+        <v>0.77950951693303683</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>0.77720623918862775</v>
+      </c>
+      <c r="R14" s="16">
+        <v>0.78232968328183516</v>
+      </c>
+      <c r="S14" s="16">
+        <v>0.80818559918137534</v>
+      </c>
+      <c r="T14" s="16">
+        <v>0.81192206987585547</v>
+      </c>
+      <c r="U14" s="16">
+        <v>0.81542208732446808</v>
+      </c>
+      <c r="V14" s="16">
+        <v>0.80074018529843705</v>
+      </c>
+      <c r="W14" s="16">
+        <v>0.75688245091261352</v>
+      </c>
+      <c r="X14" s="16">
+        <v>0.78279406819149344</v>
+      </c>
+      <c r="Y14" s="16">
+        <v>0.78471682482297511</v>
+      </c>
+      <c r="Z14" s="16">
+        <v>0.78288750995889522</v>
+      </c>
+      <c r="AA14" s="16">
+        <v>0.73190461626096071</v>
+      </c>
+      <c r="AB14" s="16">
+        <v>0.72682115743185416</v>
+      </c>
+      <c r="AC14" s="16">
+        <v>0.74216606739062985</v>
+      </c>
+      <c r="AD14" s="16">
+        <v>0.71820058696643685</v>
+      </c>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B15" s="14"/>
+      <c r="C15" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0.28798592279129132</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0.30273043443714726</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0.30659793689221654</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0.28908864348271246</v>
+      </c>
+      <c r="K15" s="16">
+        <v>0.26589751417591689</v>
+      </c>
+      <c r="L15" s="16">
+        <v>0.24293928255159269</v>
+      </c>
+      <c r="M15" s="16">
+        <v>0.25012320190567566</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0.24144837785433348</v>
+      </c>
+      <c r="O15" s="16">
+        <v>0.21095733836928579</v>
+      </c>
+      <c r="P15" s="16">
+        <v>0.20684222490251347</v>
+      </c>
+      <c r="Q15" s="16">
+        <v>0.19058245646356978</v>
+      </c>
+      <c r="R15" s="16">
+        <v>0.20350554437900714</v>
+      </c>
+      <c r="S15" s="16">
+        <v>0.19347962049581183</v>
+      </c>
+      <c r="T15" s="16">
+        <v>0.19993397774393826</v>
+      </c>
+      <c r="U15" s="16">
+        <v>0.19009771418548554</v>
+      </c>
+      <c r="V15" s="16">
+        <v>0.17146648700829201</v>
+      </c>
+      <c r="W15" s="16">
+        <v>0.17079232358359644</v>
+      </c>
+      <c r="X15" s="16">
+        <v>0.18306867617625233</v>
+      </c>
+      <c r="Y15" s="16">
+        <v>0.20611696918444519</v>
+      </c>
+      <c r="Z15" s="16">
+        <v>0.20266134589673182</v>
+      </c>
+      <c r="AA15" s="16">
+        <v>0.22588058902488387</v>
+      </c>
+      <c r="AB15" s="16">
+        <v>0.22128122885520288</v>
+      </c>
+      <c r="AC15" s="16">
+        <v>0.23174604189682166</v>
+      </c>
+      <c r="AD15" s="16">
+        <v>0.25032763782297662</v>
+      </c>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B16" s="14"/>
+      <c r="C16" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="16">
+        <v>0.11290369676699089</v>
+      </c>
+      <c r="H16" s="16">
+        <v>0.11252080497842533</v>
+      </c>
+      <c r="I16" s="16">
+        <v>0.11114392872044106</v>
+      </c>
+      <c r="J16" s="16">
+        <v>0.10980100080397107</v>
+      </c>
+      <c r="K16" s="16">
+        <v>0.10629433887348871</v>
+      </c>
+      <c r="L16" s="16">
+        <v>0.10169458996166861</v>
+      </c>
+      <c r="M16" s="16">
+        <v>0.1012474472451413</v>
+      </c>
+      <c r="N16" s="16">
+        <v>9.6250035565059594E-2</v>
+      </c>
+      <c r="O16" s="16">
+        <v>9.1116732850871171E-2</v>
+      </c>
+      <c r="P16" s="16">
+        <v>9.0705870518245663E-2</v>
+      </c>
+      <c r="Q16" s="16">
+        <v>8.907973891274662E-2</v>
+      </c>
+      <c r="R16" s="16">
+        <v>9.0774977450280667E-2</v>
+      </c>
+      <c r="S16" s="16">
+        <v>0.10621869271815901</v>
+      </c>
+      <c r="T16" s="16">
+        <v>0.1171115942875274</v>
+      </c>
+      <c r="U16" s="16">
+        <v>0.13416171440065497</v>
+      </c>
+      <c r="V16" s="16">
+        <v>0.14446583439975277</v>
+      </c>
+      <c r="W16" s="16">
+        <v>0.16426290020526127</v>
+      </c>
+      <c r="X16" s="16">
+        <v>0.15964171474487476</v>
+      </c>
+      <c r="Y16" s="16">
+        <v>0.15685583357713065</v>
+      </c>
+      <c r="Z16" s="16">
+        <v>0.1548233873178409</v>
+      </c>
+      <c r="AA16" s="16">
+        <v>0.13796149372702229</v>
+      </c>
+      <c r="AB16" s="16">
+        <v>0.13024692988354422</v>
+      </c>
+      <c r="AC16" s="16">
+        <v>0.1226331546584721</v>
+      </c>
+      <c r="AD16" s="16">
+        <v>0.12270615346495793</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+      <c r="C17" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="16">
+        <v>0.14318735144752251</v>
+      </c>
+      <c r="H17" s="16">
+        <v>0.15172814329230799</v>
+      </c>
+      <c r="I17" s="16">
+        <v>0.15286440146074756</v>
+      </c>
+      <c r="J17" s="16">
+        <v>0.14587862796586137</v>
+      </c>
+      <c r="K17" s="16">
+        <v>0.13860326243385851</v>
+      </c>
+      <c r="L17" s="16">
+        <v>0.13355937465025583</v>
+      </c>
+      <c r="M17" s="16">
+        <v>0.12390294218695391</v>
+      </c>
+      <c r="N17" s="16">
+        <v>0.11946577525353649</v>
+      </c>
+      <c r="O17" s="16">
+        <v>0.10486274320926747</v>
+      </c>
+      <c r="P17" s="16">
+        <v>9.8066026558676772E-2</v>
+      </c>
+      <c r="Q17" s="16">
+        <v>0.10063281271185989</v>
+      </c>
+      <c r="R17" s="16">
+        <v>9.935636373055165E-2</v>
+      </c>
+      <c r="S17" s="16">
+        <v>0.11025652730981667</v>
+      </c>
+      <c r="T17" s="16">
+        <v>0.1110310451095585</v>
+      </c>
+      <c r="U17" s="16">
+        <v>0.12430366819170779</v>
+      </c>
+      <c r="V17" s="16">
+        <v>0.12874767725067443</v>
+      </c>
+      <c r="W17" s="16">
+        <v>0.14110353849594359</v>
+      </c>
+      <c r="X17" s="16">
+        <v>0.14107257439660945</v>
+      </c>
+      <c r="Y17" s="16">
+        <v>0.15079603650969708</v>
+      </c>
+      <c r="Z17" s="16">
+        <v>0.15050252211472168</v>
+      </c>
+      <c r="AA17" s="16">
+        <v>0.15159692987714216</v>
+      </c>
+      <c r="AB17" s="16">
+        <v>0.14411919801194925</v>
+      </c>
+      <c r="AC17" s="16">
+        <v>0.15866862432222217</v>
+      </c>
+      <c r="AD17" s="16">
+        <v>0.15483211197229346</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="16">
+        <v>0.51621692246552908</v>
+      </c>
+      <c r="H18" s="16">
+        <v>0.53502446370907564</v>
+      </c>
+      <c r="I18" s="16">
+        <v>0.54297714117369544</v>
+      </c>
+      <c r="J18" s="16">
+        <v>0.50078613835832175</v>
+      </c>
+      <c r="K18" s="16">
+        <v>0.50792196291440317</v>
+      </c>
+      <c r="L18" s="16">
+        <v>0.49174059846586493</v>
+      </c>
+      <c r="M18" s="16">
+        <v>0.48614292958348065</v>
+      </c>
+      <c r="N18" s="16">
+        <v>0.49173184788248275</v>
+      </c>
+      <c r="O18" s="16">
+        <v>0.45160338185562826</v>
+      </c>
+      <c r="P18" s="16">
+        <v>0.46993291962596823</v>
+      </c>
+      <c r="Q18" s="16">
+        <v>0.46188182872359101</v>
+      </c>
+      <c r="R18" s="16">
+        <v>0.44859146499241931</v>
+      </c>
+      <c r="S18" s="16">
+        <v>0.42768477923825421</v>
+      </c>
+      <c r="T18" s="16">
+        <v>0.41231023056990607</v>
+      </c>
+      <c r="U18" s="16">
+        <v>0.38511386371983675</v>
+      </c>
+      <c r="V18" s="16">
+        <v>0.35665952759840686</v>
+      </c>
+      <c r="W18" s="16">
+        <v>0.34308642361296254</v>
+      </c>
+      <c r="X18" s="16">
+        <v>0.36334772522078906</v>
+      </c>
+      <c r="Y18" s="16">
+        <v>0.37208900910960963</v>
+      </c>
+      <c r="Z18" s="16">
+        <v>0.38410480410130993</v>
+      </c>
+      <c r="AA18" s="16">
+        <v>0.42108620697372268</v>
+      </c>
+      <c r="AB18" s="16">
+        <v>0.40972878989098555</v>
+      </c>
+      <c r="AC18" s="16">
+        <v>0.45629114472792565</v>
+      </c>
+      <c r="AD18" s="16">
+        <v>0.46672746772875923</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B19" s="14"/>
+      <c r="C19" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="16">
+        <v>0.32585578846809665</v>
+      </c>
+      <c r="H19" s="16">
+        <v>0.32888537954058999</v>
+      </c>
+      <c r="I19" s="16">
+        <v>0.34725819547266584</v>
+      </c>
+      <c r="J19" s="16">
+        <v>0.37480100519865422</v>
+      </c>
+      <c r="K19" s="16">
+        <v>0.39165219214300862</v>
+      </c>
+      <c r="L19" s="16">
+        <v>0.38267907485762104</v>
+      </c>
+      <c r="M19" s="16">
+        <v>0.39479240597151793</v>
+      </c>
+      <c r="N19" s="16">
+        <v>0.38185837942392092</v>
+      </c>
+      <c r="O19" s="16">
+        <v>0.42554593424251252</v>
+      </c>
+      <c r="P19" s="16">
+        <v>0.41304057693863694</v>
+      </c>
+      <c r="Q19" s="16">
+        <v>0.47577040221062672</v>
+      </c>
+      <c r="R19" s="16">
+        <v>0.45816138106597054</v>
+      </c>
+      <c r="S19" s="16">
+        <v>0.47828062330404186</v>
+      </c>
+      <c r="T19" s="16">
+        <v>0.46861155052559272</v>
+      </c>
+      <c r="U19" s="16">
+        <v>0.45299965458031333</v>
+      </c>
+      <c r="V19" s="16">
+        <v>0.44574083989683322</v>
+      </c>
+      <c r="W19" s="16">
+        <v>0.38850458117812858</v>
+      </c>
+      <c r="X19" s="16">
+        <v>0.367119374993644</v>
+      </c>
+      <c r="Y19" s="16">
+        <v>0.34623877036794248</v>
+      </c>
+      <c r="Z19" s="16">
+        <v>0.31672403049131953</v>
+      </c>
+      <c r="AA19" s="16">
+        <v>0.30012113021665487</v>
+      </c>
+      <c r="AB19" s="16">
+        <v>0.2826155137431956</v>
+      </c>
+      <c r="AC19" s="16">
+        <v>0.30428855310524533</v>
+      </c>
+      <c r="AD19" s="16">
+        <v>0.30209431447527746</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B20" s="14"/>
+      <c r="C20" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="16">
+        <v>0.53971967912593455</v>
+      </c>
+      <c r="H20" s="16">
+        <v>0.56223696727000916</v>
+      </c>
+      <c r="I20" s="16">
+        <v>0.59830631636678266</v>
+      </c>
+      <c r="J20" s="16">
+        <v>0.57196891585010479</v>
+      </c>
+      <c r="K20" s="16">
+        <v>0.62619731006802037</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0.60482058477565515</v>
+      </c>
+      <c r="M20" s="16">
+        <v>0.62059697068808761</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0.56047953389626337</v>
+      </c>
+      <c r="O20" s="16">
+        <v>0.56023937912393051</v>
+      </c>
+      <c r="P20" s="16">
+        <v>0.62331101945817813</v>
+      </c>
+      <c r="Q20" s="16">
+        <v>0.63482046899781297</v>
+      </c>
+      <c r="R20" s="16">
+        <v>0.6549426990091457</v>
+      </c>
+      <c r="S20" s="16">
+        <v>0.66575795454348108</v>
+      </c>
+      <c r="T20" s="16">
+        <v>0.66061460370309733</v>
+      </c>
+      <c r="U20" s="16">
+        <v>0.69656606519292896</v>
+      </c>
+      <c r="V20" s="16">
+        <v>0.70739420265195208</v>
+      </c>
+      <c r="W20" s="16">
+        <v>0.66456327575208807</v>
+      </c>
+      <c r="X20" s="16">
+        <v>0.68442421865427772</v>
+      </c>
+      <c r="Y20" s="16">
+        <v>0.650970098306627</v>
+      </c>
+      <c r="Z20" s="16">
+        <v>0.67158983649078929</v>
+      </c>
+      <c r="AA20" s="16">
+        <v>0.6032316217356527</v>
+      </c>
+      <c r="AB20" s="16">
+        <v>0.62668408445483081</v>
+      </c>
+      <c r="AC20" s="16">
+        <v>0.59432670861967407</v>
+      </c>
+      <c r="AD20" s="16">
+        <v>0.60509466265318956</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B21" s="14"/>
+      <c r="C21" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="16">
+        <v>0.66858608712291656</v>
+      </c>
+      <c r="H21" s="16">
+        <v>0.67742898821687103</v>
+      </c>
+      <c r="I21" s="16">
+        <v>0.70208989961616575</v>
+      </c>
+      <c r="J21" s="16">
+        <v>0.70804759553029906</v>
+      </c>
+      <c r="K21" s="16">
+        <v>0.73966621122382492</v>
+      </c>
+      <c r="L21" s="16">
+        <v>0.72341264947692574</v>
+      </c>
+      <c r="M21" s="16">
+        <v>0.74656599300897464</v>
+      </c>
+      <c r="N21" s="16">
+        <v>0.74113883178459694</v>
+      </c>
+      <c r="O21" s="16">
+        <v>0.76053781944012555</v>
+      </c>
+      <c r="P21" s="16">
+        <v>0.7944053779899094</v>
+      </c>
+      <c r="Q21" s="16">
+        <v>0.82777009712242455</v>
+      </c>
+      <c r="R21" s="16">
+        <v>0.78363400889193102</v>
+      </c>
+      <c r="S21" s="16">
+        <v>0.84188346168291661</v>
+      </c>
+      <c r="T21" s="16">
+        <v>0.79503352330568788</v>
+      </c>
+      <c r="U21" s="16">
+        <v>0.82646928515257945</v>
+      </c>
+      <c r="V21" s="16">
+        <v>0.7671255517254294</v>
+      </c>
+      <c r="W21" s="16">
+        <v>0.81815123182360328</v>
+      </c>
+      <c r="X21" s="16">
+        <v>0.77016713590538544</v>
+      </c>
+      <c r="Y21" s="16">
+        <v>0.7974487881442871</v>
+      </c>
+      <c r="Z21" s="16">
+        <v>0.72438345998617093</v>
+      </c>
+      <c r="AA21" s="16">
+        <v>0.7162392917338305</v>
+      </c>
+      <c r="AB21" s="16">
+        <v>0.75364699957365899</v>
+      </c>
+      <c r="AC21" s="16">
+        <v>0.74572531916875584</v>
+      </c>
+      <c r="AD21" s="16">
+        <v>0.74597901923411258</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B22" s="14"/>
+      <c r="C22" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="16">
+        <v>0</v>
+      </c>
+      <c r="H22" s="16">
+        <v>0</v>
+      </c>
+      <c r="I22" s="16">
+        <v>0</v>
+      </c>
+      <c r="J22" s="16">
+        <v>0</v>
+      </c>
+      <c r="K22" s="16">
+        <v>0</v>
+      </c>
+      <c r="L22" s="16">
+        <v>0</v>
+      </c>
+      <c r="M22" s="16">
+        <v>0</v>
+      </c>
+      <c r="N22" s="16">
+        <v>5.1654441096429362E-3</v>
+      </c>
+      <c r="O22" s="16">
+        <v>0.13917238651745761</v>
+      </c>
+      <c r="P22" s="16">
+        <v>0.32287667270730469</v>
+      </c>
+      <c r="Q22" s="16">
+        <v>0.46695770454946894</v>
+      </c>
+      <c r="R22" s="16">
+        <v>0.55930898011263785</v>
+      </c>
+      <c r="S22" s="16">
+        <v>0.61775152666716837</v>
+      </c>
+      <c r="T22" s="16">
+        <v>0.5715780768813592</v>
+      </c>
+      <c r="U22" s="16">
+        <v>0.43566570202843524</v>
+      </c>
+      <c r="V22" s="16">
+        <v>0.25136173668773426</v>
+      </c>
+      <c r="W22" s="16">
+        <v>5.3561400504469642E-2</v>
+      </c>
+      <c r="X22" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B23" s="14"/>
+      <c r="C23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="16">
+        <v>0</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0</v>
+      </c>
+      <c r="I23" s="16">
+        <v>0</v>
+      </c>
+      <c r="J23" s="16">
+        <v>0</v>
+      </c>
+      <c r="K23" s="16">
+        <v>0</v>
+      </c>
+      <c r="L23" s="16">
+        <v>1.5978381696877285E-2</v>
+      </c>
+      <c r="M23" s="16">
+        <v>0.12054041363174194</v>
+      </c>
+      <c r="N23" s="16">
+        <v>0.29299121495912761</v>
+      </c>
+      <c r="O23" s="16">
+        <v>0.51249664727039823</v>
+      </c>
+      <c r="P23" s="16">
+        <v>0.68999283771675057</v>
+      </c>
+      <c r="Q23" s="16">
+        <v>0.75711785971351131</v>
+      </c>
+      <c r="R23" s="16">
+        <v>0.86419769400114987</v>
+      </c>
+      <c r="S23" s="16">
+        <v>0.83120736472782852</v>
+      </c>
+      <c r="T23" s="16">
+        <v>0.75687258072072439</v>
+      </c>
+      <c r="U23" s="16">
+        <v>0.66049436245582582</v>
+      </c>
+      <c r="V23" s="16">
+        <v>0.51733953268421395</v>
+      </c>
+      <c r="W23" s="16">
+        <v>0.33627659412719996</v>
+      </c>
+      <c r="X23" s="16">
+        <v>0.17073889633423281</v>
+      </c>
+      <c r="Y23" s="16">
+        <v>4.6327441455081442E-2</v>
+      </c>
+      <c r="Z23" s="16">
+        <v>1.5464912013420456E-3</v>
+      </c>
+      <c r="AA23" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B24" s="14"/>
+      <c r="C24" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="16">
+        <v>0</v>
+      </c>
+      <c r="H24" s="16">
+        <v>0</v>
+      </c>
+      <c r="I24" s="16">
+        <v>0</v>
+      </c>
+      <c r="J24" s="16">
+        <v>0</v>
+      </c>
+      <c r="K24" s="16">
+        <v>0</v>
+      </c>
+      <c r="L24" s="16">
+        <v>5.8022640849951252E-4</v>
+      </c>
+      <c r="M24" s="16">
+        <v>4.1860052067493082E-2</v>
+      </c>
+      <c r="N24" s="16">
+        <v>0.19802038717986975</v>
+      </c>
+      <c r="O24" s="16">
+        <v>0.38901600821190918</v>
+      </c>
+      <c r="P24" s="16">
+        <v>0.58552237969413967</v>
+      </c>
+      <c r="Q24" s="16">
+        <v>0.75069907281169146</v>
+      </c>
+      <c r="R24" s="16">
+        <v>0.74953660430870916</v>
+      </c>
+      <c r="S24" s="16">
+        <v>0.82814244459051434</v>
+      </c>
+      <c r="T24" s="16">
+        <v>0.74747123131360205</v>
+      </c>
+      <c r="U24" s="16">
+        <v>0.61024966672790093</v>
+      </c>
+      <c r="V24" s="16">
+        <v>0.4434897616780541</v>
+      </c>
+      <c r="W24" s="16">
+        <v>0.27362901503500309</v>
+      </c>
+      <c r="X24" s="16">
+        <v>9.3437163457212508E-2</v>
+      </c>
+      <c r="Y24" s="16">
+        <v>6.8682831944611522E-3</v>
+      </c>
+      <c r="Z24" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B25" s="14"/>
+      <c r="C25" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="16">
+        <v>0</v>
+      </c>
+      <c r="H25" s="16">
+        <v>0</v>
+      </c>
+      <c r="I25" s="16">
+        <v>0</v>
+      </c>
+      <c r="J25" s="16">
+        <v>0</v>
+      </c>
+      <c r="K25" s="16">
+        <v>0</v>
+      </c>
+      <c r="L25" s="16">
+        <v>2.0682373217113158E-4</v>
+      </c>
+      <c r="M25" s="16">
+        <v>8.9382337865689596E-3</v>
+      </c>
+      <c r="N25" s="16">
+        <v>6.9681743636966012E-2</v>
+      </c>
+      <c r="O25" s="16">
+        <v>0.19744222413309606</v>
+      </c>
+      <c r="P25" s="16">
+        <v>0.37498439611881212</v>
+      </c>
+      <c r="Q25" s="16">
+        <v>0.47918948939036954</v>
+      </c>
+      <c r="R25" s="16">
+        <v>0.59059635444130043</v>
+      </c>
+      <c r="S25" s="16">
+        <v>0.56574325133432102</v>
+      </c>
+      <c r="T25" s="16">
+        <v>0.53549409918373392</v>
+      </c>
+      <c r="U25" s="16">
+        <v>0.42611239841079246</v>
+      </c>
+      <c r="V25" s="16">
+        <v>0.29819583256754928</v>
+      </c>
+      <c r="W25" s="16">
+        <v>0.13151978303785003</v>
+      </c>
+      <c r="X25" s="16">
+        <v>2.6467917658707589E-2</v>
+      </c>
+      <c r="Y25" s="16">
+        <v>2.0345163747184365E-3</v>
+      </c>
+      <c r="Z25" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B26" s="14"/>
+      <c r="C26" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="16">
+        <v>0</v>
+      </c>
+      <c r="H26" s="16">
+        <v>0</v>
+      </c>
+      <c r="I26" s="16">
+        <v>0</v>
+      </c>
+      <c r="J26" s="16">
+        <v>0</v>
+      </c>
+      <c r="K26" s="16">
+        <v>0</v>
+      </c>
+      <c r="L26" s="16">
+        <v>1.7222430132224097E-2</v>
+      </c>
+      <c r="M26" s="16">
+        <v>0.11874718290139995</v>
+      </c>
+      <c r="N26" s="16">
+        <v>0.29501274681029421</v>
+      </c>
+      <c r="O26" s="16">
+        <v>0.5099280039617321</v>
+      </c>
+      <c r="P26" s="16">
+        <v>0.67375186313201152</v>
+      </c>
+      <c r="Q26" s="16">
+        <v>0.7937659472480465</v>
+      </c>
+      <c r="R26" s="16">
+        <v>0.86462403872224325</v>
+      </c>
+      <c r="S26" s="16">
+        <v>0.87726536249905551</v>
+      </c>
+      <c r="T26" s="16">
+        <v>0.80024733163330863</v>
+      </c>
+      <c r="U26" s="16">
+        <v>0.71886660572990679</v>
+      </c>
+      <c r="V26" s="16">
+        <v>0.54881311814175615</v>
+      </c>
+      <c r="W26" s="16">
+        <v>0.35366624767547827</v>
+      </c>
+      <c r="X26" s="16">
+        <v>0.1773736692645714</v>
+      </c>
+      <c r="Y26" s="16">
+        <v>5.1813045923291459E-2</v>
+      </c>
+      <c r="Z26" s="16">
+        <v>2.0524245049981732E-3</v>
+      </c>
+      <c r="AA26" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B27" s="14"/>
+      <c r="C27" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="16">
+        <v>0</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0</v>
+      </c>
+      <c r="I27" s="16">
+        <v>0</v>
+      </c>
+      <c r="J27" s="16">
+        <v>0</v>
+      </c>
+      <c r="K27" s="16">
+        <v>0</v>
+      </c>
+      <c r="L27" s="16">
+        <v>0</v>
+      </c>
+      <c r="M27" s="16">
+        <v>0</v>
+      </c>
+      <c r="N27" s="16">
+        <v>5.4549486394356835E-3</v>
+      </c>
+      <c r="O27" s="16">
+        <v>0.11661301892658829</v>
+      </c>
+      <c r="P27" s="16">
+        <v>0.28892093789037271</v>
+      </c>
+      <c r="Q27" s="16">
+        <v>0.42860309799611129</v>
+      </c>
+      <c r="R27" s="16">
+        <v>0.51377193607510041</v>
+      </c>
+      <c r="S27" s="16">
+        <v>0.52969762313614988</v>
+      </c>
+      <c r="T27" s="16">
+        <v>0.49334059758142462</v>
+      </c>
+      <c r="U27" s="16">
+        <v>0.39560811862067191</v>
+      </c>
+      <c r="V27" s="16">
+        <v>0.24316146294571353</v>
+      </c>
+      <c r="W27" s="16">
+        <v>4.9257665793127653E-2</v>
+      </c>
+      <c r="X27" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B28" s="14"/>
+      <c r="C28" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="16">
+        <v>0</v>
+      </c>
+      <c r="H28" s="16">
+        <v>0</v>
+      </c>
+      <c r="I28" s="16">
+        <v>0</v>
+      </c>
+      <c r="J28" s="16">
+        <v>0</v>
+      </c>
+      <c r="K28" s="16">
+        <v>0</v>
+      </c>
+      <c r="L28" s="16">
+        <v>4.9619385853992147E-4</v>
+      </c>
+      <c r="M28" s="16">
+        <v>7.4009008291900215E-3</v>
+      </c>
+      <c r="N28" s="16">
+        <v>5.0475805781788188E-2</v>
+      </c>
+      <c r="O28" s="16">
+        <v>0.16453512102199117</v>
+      </c>
+      <c r="P28" s="16">
+        <v>0.30543884718105085</v>
+      </c>
+      <c r="Q28" s="16">
+        <v>0.44123794847349379</v>
+      </c>
+      <c r="R28" s="16">
+        <v>0.50640982862433559</v>
+      </c>
+      <c r="S28" s="16">
+        <v>0.53923292542204859</v>
+      </c>
+      <c r="T28" s="16">
+        <v>0.50011663543860208</v>
+      </c>
+      <c r="U28" s="16">
+        <v>0.39882913916590412</v>
+      </c>
+      <c r="V28" s="16">
+        <v>0.26363931143128477</v>
+      </c>
+      <c r="W28" s="16">
+        <v>9.87689962911278E-2</v>
+      </c>
+      <c r="X28" s="16">
+        <v>1.6859931262641237E-2</v>
+      </c>
+      <c r="Y28" s="16">
+        <v>2.3880901278652577E-3</v>
+      </c>
+      <c r="Z28" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B29" s="14"/>
+      <c r="C29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="16">
+        <v>0</v>
+      </c>
+      <c r="H29" s="16">
+        <v>0</v>
+      </c>
+      <c r="I29" s="16">
+        <v>0</v>
+      </c>
+      <c r="J29" s="16">
+        <v>0</v>
+      </c>
+      <c r="K29" s="16">
+        <v>0</v>
+      </c>
+      <c r="L29" s="16">
+        <v>0</v>
+      </c>
+      <c r="M29" s="16">
+        <v>0</v>
+      </c>
+      <c r="N29" s="16">
+        <v>4.9964528059104679E-3</v>
+      </c>
+      <c r="O29" s="16">
+        <v>0.13548453868278298</v>
+      </c>
+      <c r="P29" s="16">
+        <v>0.32392518396834408</v>
+      </c>
+      <c r="Q29" s="16">
+        <v>0.4965122705763827</v>
+      </c>
+      <c r="R29" s="16">
+        <v>0.57211223710463355</v>
+      </c>
+      <c r="S29" s="16">
+        <v>0.56577785956427906</v>
+      </c>
+      <c r="T29" s="16">
+        <v>0.57341598898861423</v>
+      </c>
+      <c r="U29" s="16">
+        <v>0.42276820161479362</v>
+      </c>
+      <c r="V29" s="16">
+        <v>0.25325765812858164</v>
+      </c>
+      <c r="W29" s="16">
+        <v>5.7498679454463388E-2</v>
+      </c>
+      <c r="X29" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B30" s="14"/>
+      <c r="C30" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="16">
+        <v>0</v>
+      </c>
+      <c r="H30" s="16">
+        <v>0</v>
+      </c>
+      <c r="I30" s="16">
+        <v>0</v>
+      </c>
+      <c r="J30" s="16">
+        <v>0</v>
+      </c>
+      <c r="K30" s="16">
+        <v>0</v>
+      </c>
+      <c r="L30" s="16">
+        <v>1.6005714906171902E-2</v>
+      </c>
+      <c r="M30" s="16">
+        <v>0.11218533781286343</v>
+      </c>
+      <c r="N30" s="16">
+        <v>0.3064455042278465</v>
+      </c>
+      <c r="O30" s="16">
+        <v>0.48857009117639782</v>
+      </c>
+      <c r="P30" s="16">
+        <v>0.64972862153275091</v>
+      </c>
+      <c r="Q30" s="16">
+        <v>0.78951215089545324</v>
+      </c>
+      <c r="R30" s="16">
+        <v>0.85898717174770867</v>
+      </c>
+      <c r="S30" s="16">
+        <v>0.79158938800905354</v>
+      </c>
+      <c r="T30" s="16">
+        <v>0.79321713098771129</v>
+      </c>
+      <c r="U30" s="16">
+        <v>0.65318838320718775</v>
+      </c>
+      <c r="V30" s="16">
+        <v>0.55667724349067083</v>
+      </c>
+      <c r="W30" s="16">
+        <v>0.34301226873361118</v>
+      </c>
+      <c r="X30" s="16">
+        <v>0.16475726961604273</v>
+      </c>
+      <c r="Y30" s="16">
+        <v>4.5348478929008521E-2</v>
+      </c>
+      <c r="Z30" s="16">
+        <v>1.5832235105023565E-3</v>
+      </c>
+      <c r="AA30" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B31" s="14"/>
+      <c r="C31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="16">
+        <v>0</v>
+      </c>
+      <c r="H31" s="16">
+        <v>0</v>
+      </c>
+      <c r="I31" s="16">
+        <v>0</v>
+      </c>
+      <c r="J31" s="16">
+        <v>0</v>
+      </c>
+      <c r="K31" s="16">
+        <v>0</v>
+      </c>
+      <c r="L31" s="16">
+        <v>5.9562326159201518E-4</v>
+      </c>
+      <c r="M31" s="16">
+        <v>3.9641182771296531E-2</v>
+      </c>
+      <c r="N31" s="16">
+        <v>0.20352127834130515</v>
+      </c>
+      <c r="O31" s="16">
+        <v>0.41942365678109861</v>
+      </c>
+      <c r="P31" s="16">
+        <v>0.59252759645876873</v>
+      </c>
+      <c r="Q31" s="16">
+        <v>0.73225592185519428</v>
+      </c>
+      <c r="R31" s="16">
+        <v>0.75164897706759426</v>
+      </c>
+      <c r="S31" s="16">
+        <v>0.77168296614129095</v>
+      </c>
+      <c r="T31" s="16">
+        <v>0.75500033997653926</v>
+      </c>
+      <c r="U31" s="16">
+        <v>0.6506014013878425</v>
+      </c>
+      <c r="V31" s="16">
+        <v>0.44209566281281554</v>
+      </c>
+      <c r="W31" s="16">
+        <v>0.27369136957266599</v>
+      </c>
+      <c r="X31" s="16">
+        <v>9.543046901502257E-2</v>
+      </c>
+      <c r="Y31" s="16">
+        <v>7.1583534977902666E-3</v>
+      </c>
+      <c r="Z31" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B32" s="14"/>
+      <c r="C32" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="16">
+        <v>0</v>
+      </c>
+      <c r="H32" s="16">
+        <v>0</v>
+      </c>
+      <c r="I32" s="16">
+        <v>0</v>
+      </c>
+      <c r="J32" s="16">
+        <v>0</v>
+      </c>
+      <c r="K32" s="16">
+        <v>0</v>
+      </c>
+      <c r="L32" s="16">
+        <v>2.0473031458811933E-4</v>
+      </c>
+      <c r="M32" s="16">
+        <v>8.6080648917654639E-3</v>
+      </c>
+      <c r="N32" s="16">
+        <v>6.7093607585111334E-2</v>
+      </c>
+      <c r="O32" s="16">
+        <v>0.19614861974762729</v>
+      </c>
+      <c r="P32" s="16">
+        <v>0.36567611414802786</v>
+      </c>
+      <c r="Q32" s="16">
+        <v>0.47700100357601033</v>
+      </c>
+      <c r="R32" s="16">
+        <v>0.55012669514917412</v>
+      </c>
+      <c r="S32" s="16">
+        <v>0.56488703705636834</v>
+      </c>
+      <c r="T32" s="16">
+        <v>0.53903204225003909</v>
+      </c>
+      <c r="U32" s="16">
+        <v>0.44243036783146034</v>
+      </c>
+      <c r="V32" s="16">
+        <v>0.29785267272201932</v>
+      </c>
+      <c r="W32" s="16">
+        <v>0.13482113824013897</v>
+      </c>
+      <c r="X32" s="16">
+        <v>2.7222907612690042E-2</v>
+      </c>
+      <c r="Y32" s="16">
+        <v>2.1004834314281907E-3</v>
+      </c>
+      <c r="Z32" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B33" s="14"/>
+      <c r="C33" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="16">
+        <v>0</v>
+      </c>
+      <c r="H33" s="16">
+        <v>0</v>
+      </c>
+      <c r="I33" s="16">
+        <v>0</v>
+      </c>
+      <c r="J33" s="16">
+        <v>0</v>
+      </c>
+      <c r="K33" s="16">
+        <v>0</v>
+      </c>
+      <c r="L33" s="16">
+        <v>1.7145845908496556E-2</v>
+      </c>
+      <c r="M33" s="16">
+        <v>0.12084022666198764</v>
+      </c>
+      <c r="N33" s="16">
+        <v>0.29415929927779028</v>
+      </c>
+      <c r="O33" s="16">
+        <v>0.52644538731961121</v>
+      </c>
+      <c r="P33" s="16">
+        <v>0.65485791752035805</v>
+      </c>
+      <c r="Q33" s="16">
+        <v>0.81910974144062509</v>
+      </c>
+      <c r="R33" s="16">
+        <v>0.82077065712679198</v>
+      </c>
+      <c r="S33" s="16">
+        <v>0.82563252922714692</v>
+      </c>
+      <c r="T33" s="16">
+        <v>0.807752328837263</v>
+      </c>
+      <c r="U33" s="16">
+        <v>0.69488000191069133</v>
+      </c>
+      <c r="V33" s="16">
+        <v>0.54569340957868195</v>
+      </c>
+      <c r="W33" s="16">
+        <v>0.37751483261896468</v>
+      </c>
+      <c r="X33" s="16">
+        <v>0.17023410824726182</v>
+      </c>
+      <c r="Y33" s="16">
+        <v>5.1808739235912074E-2</v>
+      </c>
+      <c r="Z33" s="16">
+        <v>2.1406871368041314E-3</v>
+      </c>
+      <c r="AA33" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B34" s="14"/>
+      <c r="C34" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="16">
+        <v>0</v>
+      </c>
+      <c r="H34" s="16">
+        <v>0</v>
+      </c>
+      <c r="I34" s="16">
+        <v>0</v>
+      </c>
+      <c r="J34" s="16">
+        <v>0</v>
+      </c>
+      <c r="K34" s="16">
+        <v>0</v>
+      </c>
+      <c r="L34" s="16">
+        <v>0</v>
+      </c>
+      <c r="M34" s="16">
+        <v>0</v>
+      </c>
+      <c r="N34" s="16">
+        <v>5.1411847237239523E-3</v>
+      </c>
+      <c r="O34" s="16">
+        <v>0.11190480369868666</v>
+      </c>
+      <c r="P34" s="16">
+        <v>0.27357011551648253</v>
+      </c>
+      <c r="Q34" s="16">
+        <v>0.41277770392548069</v>
+      </c>
+      <c r="R34" s="16">
+        <v>0.50551733982214297</v>
+      </c>
+      <c r="S34" s="16">
+        <v>0.53991733626568761</v>
+      </c>
+      <c r="T34" s="16">
+        <v>0.47525531461660009</v>
+      </c>
+      <c r="U34" s="16">
+        <v>0.40797193810932164</v>
+      </c>
+      <c r="V34" s="16">
+        <v>0.23628994055123154</v>
+      </c>
+      <c r="W34" s="16">
+        <v>4.9319437880456896E-2</v>
+      </c>
+      <c r="X34" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="16">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B35" s="14"/>
+      <c r="C35" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="16">
+        <v>0</v>
+      </c>
+      <c r="H35" s="16">
+        <v>0</v>
+      </c>
+      <c r="I35" s="16">
+        <v>0</v>
+      </c>
+      <c r="J35" s="16">
+        <v>0</v>
+      </c>
+      <c r="K35" s="16">
+        <v>0</v>
+      </c>
+      <c r="L35" s="16">
+        <v>5.2440244822270926E-4</v>
+      </c>
+      <c r="M35" s="16">
+        <v>7.5212581468510845E-3</v>
+      </c>
+      <c r="N35" s="16">
+        <v>5.1973898575636224E-2</v>
+      </c>
+      <c r="O35" s="16">
+        <v>0.17284934020150328</v>
+      </c>
+      <c r="P35" s="16">
+        <v>0.30205516340235422</v>
+      </c>
+      <c r="Q35" s="16">
+        <v>0.44202745194599619</v>
+      </c>
+      <c r="R35" s="16">
+        <v>0.50631043932438557</v>
+      </c>
+      <c r="S35" s="16">
+        <v>0.52722251775143436</v>
+      </c>
+      <c r="T35" s="16">
+        <v>0.46343613801975236</v>
+      </c>
+      <c r="U35" s="16">
+        <v>0.39564512288099724</v>
+      </c>
+      <c r="V35" s="16">
+        <v>0.2586520700402351</v>
+      </c>
+      <c r="W35" s="16">
+        <v>0.10292170997118238</v>
+      </c>
+      <c r="X35" s="16">
+        <v>1.6442614411001231E-2</v>
+      </c>
+      <c r="Y35" s="16">
+        <v>2.4109186324544605E-3</v>
+      </c>
+      <c r="Z35" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4"/>
+      <c r="AA37" s="4"/>
+      <c r="AB37" s="4"/>
+      <c r="AC37" s="4"/>
+    </row>
+    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
+      <c r="Z38" s="4"/>
+      <c r="AA38" s="4"/>
+      <c r="AB38" s="4"/>
+      <c r="AC38" s="4"/>
+    </row>
+    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="4"/>
+      <c r="AA39" s="4"/>
+      <c r="AB39" s="4"/>
+      <c r="AC39" s="4"/>
+    </row>
+    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+      <c r="W40" s="4"/>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="4"/>
+      <c r="Z40" s="4"/>
+      <c r="AA40" s="4"/>
+      <c r="AB40" s="4"/>
+      <c r="AC40" s="4"/>
+    </row>
+    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="4"/>
+      <c r="Z41" s="4"/>
+      <c r="AA41" s="4"/>
+      <c r="AB41" s="4"/>
+      <c r="AC41" s="4"/>
+    </row>
+    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="4"/>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4"/>
+      <c r="AB42" s="4"/>
+      <c r="AC42" s="4"/>
+    </row>
+    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4"/>
+      <c r="AB43" s="4"/>
+      <c r="AC43" s="4"/>
+    </row>
+    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C44" s="5"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="4"/>
+      <c r="Y44" s="4"/>
+      <c r="Z44" s="4"/>
+      <c r="AA44" s="4"/>
+      <c r="AB44" s="4"/>
+      <c r="AC44" s="4"/>
+    </row>
+    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
+      <c r="AA45" s="4"/>
+      <c r="AB45" s="4"/>
+      <c r="AC45" s="4"/>
+    </row>
+    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C46" s="5"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4"/>
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="4"/>
+    </row>
+    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C47" s="5"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
+      <c r="X47" s="4"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="4"/>
+      <c r="AA47" s="4"/>
+      <c r="AB47" s="4"/>
+      <c r="AC47" s="4"/>
+    </row>
+    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="C48" s="5"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="4"/>
+      <c r="X48" s="4"/>
+      <c r="Y48" s="4"/>
+      <c r="Z48" s="4"/>
+      <c r="AA48" s="4"/>
+      <c r="AB48" s="4"/>
+      <c r="AC48" s="4"/>
+    </row>
+    <row r="49" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C49" s="5"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="4"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+      <c r="AB49" s="4"/>
+      <c r="AC49" s="4"/>
+    </row>
+    <row r="50" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C50" s="5"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="4"/>
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
+      <c r="AA50" s="4"/>
+      <c r="AB50" s="4"/>
+      <c r="AC50" s="4"/>
+    </row>
+    <row r="51" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C51" s="5"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4"/>
+      <c r="W51" s="4"/>
+      <c r="X51" s="4"/>
+      <c r="Y51" s="4"/>
+      <c r="Z51" s="4"/>
+      <c r="AA51" s="4"/>
+      <c r="AB51" s="4"/>
+      <c r="AC51" s="4"/>
+    </row>
+    <row r="52" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C52" s="5"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4"/>
+      <c r="X52" s="4"/>
+      <c r="Y52" s="4"/>
+      <c r="Z52" s="4"/>
+      <c r="AA52" s="4"/>
+      <c r="AB52" s="4"/>
+      <c r="AC52" s="4"/>
+    </row>
+    <row r="53" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C53" s="5"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="4"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="4"/>
+      <c r="W53" s="4"/>
+      <c r="X53" s="4"/>
+      <c r="Y53" s="4"/>
+      <c r="Z53" s="4"/>
+      <c r="AA53" s="4"/>
+      <c r="AB53" s="4"/>
+      <c r="AC53" s="4"/>
+    </row>
+    <row r="54" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C54" s="5"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="4"/>
+      <c r="X54" s="4"/>
+      <c r="Y54" s="4"/>
+      <c r="Z54" s="4"/>
+      <c r="AA54" s="4"/>
+      <c r="AB54" s="4"/>
+      <c r="AC54" s="4"/>
+    </row>
+    <row r="55" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C55" s="5"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+      <c r="W55" s="4"/>
+      <c r="X55" s="4"/>
+      <c r="Y55" s="4"/>
+      <c r="Z55" s="4"/>
+      <c r="AA55" s="4"/>
+      <c r="AB55" s="4"/>
+      <c r="AC55" s="4"/>
+    </row>
+    <row r="56" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C56" s="5"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4"/>
+      <c r="Z56" s="4"/>
+      <c r="AA56" s="4"/>
+      <c r="AB56" s="4"/>
+      <c r="AC56" s="4"/>
+    </row>
+    <row r="57" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C57" s="5"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="4"/>
+      <c r="X57" s="4"/>
+      <c r="Y57" s="4"/>
+      <c r="Z57" s="4"/>
+      <c r="AA57" s="4"/>
+      <c r="AB57" s="4"/>
+      <c r="AC57" s="4"/>
+    </row>
+    <row r="58" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C58" s="5"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="4"/>
+      <c r="X58" s="4"/>
+      <c r="Y58" s="4"/>
+      <c r="Z58" s="4"/>
+      <c r="AA58" s="4"/>
+      <c r="AB58" s="4"/>
+      <c r="AC58" s="4"/>
+    </row>
+    <row r="59" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C59" s="5"/>
+    </row>
+    <row r="60" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C60" s="5"/>
+    </row>
+    <row r="61" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C61" s="5"/>
+    </row>
+    <row r="62" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C62" s="5"/>
+    </row>
+    <row r="63" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C63" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4552,26 +8143,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4595,9 +8175,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>